<commit_message>
Adding the Intraday Model for Imperial
</commit_message>
<xml_diff>
--- a/Imperial/Real-Time_forecast_dataset.xlsx
+++ b/Imperial/Real-Time_forecast_dataset.xlsx
@@ -34,292 +34,292 @@
     <t>Energy_MWh</t>
   </si>
   <si>
-    <t>2024-06-19 00:00:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 00:15:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 00:30:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 00:45:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 01:00:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 01:15:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 01:30:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 01:45:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 02:00:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 02:15:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 02:30:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 02:45:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 03:00:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 03:15:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 03:30:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 03:45:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 04:00:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 04:15:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 04:30:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 04:45:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 05:00:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 05:15:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 05:30:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 05:45:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 06:00:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 06:15:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 06:30:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 06:45:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 07:00:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 07:15:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 07:30:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 07:45:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 08:00:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 08:15:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 08:30:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 08:45:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 09:00:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 09:15:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 09:30:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 09:45:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 10:00:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 10:15:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 10:30:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 10:45:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 11:00:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 11:15:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 11:30:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 11:45:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 12:00:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 12:15:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 12:30:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 12:45:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 13:00:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 13:15:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 13:30:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 13:45:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 14:00:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 14:15:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 14:30:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 14:45:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 15:00:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 15:15:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 15:30:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 15:45:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 16:00:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 16:15:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 16:30:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 16:45:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 17:00:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 17:15:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 17:30:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 17:45:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 18:00:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 18:15:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 18:30:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 18:45:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 19:00:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 19:15:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 19:30:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 19:45:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 20:00:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 20:15:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 20:30:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 20:45:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 21:00:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 21:15:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 21:30:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 21:45:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 22:00:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 22:15:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 22:30:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 22:45:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 23:00:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 23:15:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 23:30:00+00:00</t>
-  </si>
-  <si>
-    <t>2024-06-19 23:45:00+00:00</t>
+    <t>2024-06-20 00:00:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 00:15:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 00:30:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 00:45:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 01:00:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 01:15:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 01:30:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 01:45:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 02:00:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 02:15:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 02:30:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 02:45:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 03:00:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 03:15:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 03:30:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 03:45:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 04:00:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 04:15:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 04:30:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 04:45:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 05:00:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 05:15:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 05:30:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 05:45:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 06:00:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 06:15:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 06:30:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 06:45:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 07:00:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 07:15:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 07:30:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 07:45:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 08:00:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 08:15:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 08:30:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 08:45:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 09:00:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 09:15:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 09:30:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 09:45:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 10:00:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 10:15:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 10:30:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 10:45:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 11:00:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 11:15:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 11:30:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 11:45:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 12:00:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 12:15:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 12:30:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 12:45:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 13:00:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 13:15:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 13:30:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 13:45:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 14:00:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 14:15:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 14:30:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 14:45:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 15:00:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 15:15:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 15:30:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 15:45:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 16:00:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 16:15:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 16:30:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 16:45:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 17:00:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 17:15:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 17:30:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 17:45:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 18:00:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 18:15:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 18:30:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 18:45:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 19:00:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 19:15:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 19:30:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 19:45:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 20:00:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 20:15:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 20:30:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 20:45:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 21:00:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 21:15:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 21:30:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 21:45:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 22:00:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 22:15:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 22:30:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 22:45:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 23:00:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 23:15:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 23:30:00+00:00</t>
+  </si>
+  <si>
+    <t>2024-06-20 23:45:00+00:00</t>
   </si>
 </sst>
 </file>
@@ -1139,19 +1139,19 @@
         <v>28</v>
       </c>
       <c r="B24">
-        <v>689.099866231283</v>
+        <v>477.319564819336</v>
       </c>
       <c r="C24">
-        <v>0.0006890998662312</v>
+        <v>0.0004773195648193</v>
       </c>
       <c r="D24">
         <v>0</v>
       </c>
       <c r="E24">
-        <v>0.0003445499331156</v>
+        <v>0.0002386597824096</v>
       </c>
       <c r="F24">
-        <v>8.613748327891039E-05</v>
+        <v>5.9664945602417E-05</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1159,19 +1159,19 @@
         <v>29</v>
       </c>
       <c r="B25">
-        <v>7859.702987670898</v>
+        <v>9669.322886149088</v>
       </c>
       <c r="C25">
-        <v>0.007859702987670801</v>
+        <v>0.009669322886149001</v>
       </c>
       <c r="D25">
-        <v>0.0006890998662312</v>
+        <v>0.0004773195648193</v>
       </c>
       <c r="E25">
-        <v>0.004274401426951</v>
+        <v>0.0050733212254842</v>
       </c>
       <c r="F25">
-        <v>0.0010686003567377</v>
+        <v>0.001268330306371</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1179,19 +1179,19 @@
         <v>30</v>
       </c>
       <c r="B26">
-        <v>21855.46544392904</v>
+        <v>22303.94885253906</v>
       </c>
       <c r="C26">
-        <v>0.021855465443929</v>
+        <v>0.022303948852539</v>
       </c>
       <c r="D26">
-        <v>0.007859702987670801</v>
+        <v>0.009669322886149001</v>
       </c>
       <c r="E26">
-        <v>0.0148575842157999</v>
+        <v>0.015986635869344</v>
       </c>
       <c r="F26">
-        <v>0.0037143960539499</v>
+        <v>0.003996658967336</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1199,19 +1199,19 @@
         <v>31</v>
       </c>
       <c r="B27">
-        <v>47716.76338704427</v>
+        <v>47434.49605305989</v>
       </c>
       <c r="C27">
-        <v>0.0477167633870442</v>
+        <v>0.0474344960530598</v>
       </c>
       <c r="D27">
-        <v>0.021855465443929</v>
+        <v>0.022303948852539</v>
       </c>
       <c r="E27">
-        <v>0.0347861144154866</v>
+        <v>0.0348692224527994</v>
       </c>
       <c r="F27">
-        <v>0.008696528603871601</v>
+        <v>0.0087173056131998</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1219,19 +1219,19 @@
         <v>32</v>
       </c>
       <c r="B28">
-        <v>66857.48278808594</v>
+        <v>79177.75773111981</v>
       </c>
       <c r="C28">
-        <v>0.0668574827880859</v>
+        <v>0.07917775773111971</v>
       </c>
       <c r="D28">
-        <v>0.0477167633870442</v>
+        <v>0.0474344960530598</v>
       </c>
       <c r="E28">
-        <v>0.057287123087565</v>
+        <v>0.0633061268920897</v>
       </c>
       <c r="F28">
-        <v>0.0143217807718912</v>
+        <v>0.0158265317230223</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1239,19 +1239,19 @@
         <v>33</v>
       </c>
       <c r="B29">
-        <v>86289.01322428384</v>
+        <v>124548.9918619792</v>
       </c>
       <c r="C29">
-        <v>0.0862890132242838</v>
+        <v>0.1245489918619791</v>
       </c>
       <c r="D29">
-        <v>0.0668574827880859</v>
+        <v>0.07917775773111971</v>
       </c>
       <c r="E29">
-        <v>0.0765732480061848</v>
+        <v>0.1018633747965493</v>
       </c>
       <c r="F29">
-        <v>0.0191433120015461</v>
+        <v>0.0254658436991372</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1259,19 +1259,19 @@
         <v>34</v>
       </c>
       <c r="B30">
-        <v>130161.9264322917</v>
+        <v>153450.9052734375</v>
       </c>
       <c r="C30">
-        <v>0.1301619264322915</v>
+        <v>0.1534509052734374</v>
       </c>
       <c r="D30">
-        <v>0.0862890132242838</v>
+        <v>0.1245489918619791</v>
       </c>
       <c r="E30">
-        <v>0.1082254698282877</v>
+        <v>0.1389999485677083</v>
       </c>
       <c r="F30">
-        <v>0.0270563674570719</v>
+        <v>0.034749987141927</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1279,19 +1279,19 @@
         <v>35</v>
       </c>
       <c r="B31">
-        <v>229625.5572102864</v>
+        <v>265880.1848958333</v>
       </c>
       <c r="C31">
-        <v>0.2296255572102864</v>
+        <v>0.2658801848958333</v>
       </c>
       <c r="D31">
-        <v>0.1301619264322915</v>
+        <v>0.1534509052734374</v>
       </c>
       <c r="E31">
-        <v>0.179893741821289</v>
+        <v>0.2096655450846353</v>
       </c>
       <c r="F31">
-        <v>0.0449734354553222</v>
+        <v>0.0524163862711587</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1299,19 +1299,19 @@
         <v>36</v>
       </c>
       <c r="B32">
-        <v>386699.9888509115</v>
+        <v>403181.9327799479</v>
       </c>
       <c r="C32">
-        <v>0.3866999888509115</v>
+        <v>0.4031819327799478</v>
       </c>
       <c r="D32">
-        <v>0.2296255572102864</v>
+        <v>0.2658801848958333</v>
       </c>
       <c r="E32">
-        <v>0.3081627730305988</v>
+        <v>0.3345310588378905</v>
       </c>
       <c r="F32">
-        <v>0.0770406932576496</v>
+        <v>0.08363276470947259</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1319,19 +1319,19 @@
         <v>37</v>
       </c>
       <c r="B33">
-        <v>594515.7807617188</v>
+        <v>560271.0364583333</v>
       </c>
       <c r="C33">
-        <v>0.5945157807617187</v>
+        <v>0.5602710364583333</v>
       </c>
       <c r="D33">
-        <v>0.3866999888509115</v>
+        <v>0.4031819327799478</v>
       </c>
       <c r="E33">
-        <v>0.4906078848063151</v>
+        <v>0.4817264846191405</v>
       </c>
       <c r="F33">
-        <v>0.1226519712015787</v>
+        <v>0.120431621154785</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1339,19 +1339,19 @@
         <v>38</v>
       </c>
       <c r="B34">
-        <v>803619.599609375</v>
+        <v>742276.8916015625</v>
       </c>
       <c r="C34">
-        <v>0.8036195996093749</v>
+        <v>0.7422768916015624</v>
       </c>
       <c r="D34">
-        <v>0.5945157807617187</v>
+        <v>0.5602710364583333</v>
       </c>
       <c r="E34">
-        <v>0.6990676901855467</v>
+        <v>0.6512739640299479</v>
       </c>
       <c r="F34">
-        <v>0.1747669225463866</v>
+        <v>0.1628184910074869</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1359,19 +1359,19 @@
         <v>39</v>
       </c>
       <c r="B35">
-        <v>1028912.063802083</v>
+        <v>942833.2473958333</v>
       </c>
       <c r="C35">
-        <v>1.028912063802083</v>
+        <v>0.9428332473958332</v>
       </c>
       <c r="D35">
-        <v>0.8036195996093749</v>
+        <v>0.7422768916015624</v>
       </c>
       <c r="E35">
-        <v>0.9162658317057291</v>
+        <v>0.8425550694986979</v>
       </c>
       <c r="F35">
-        <v>0.2290664579264322</v>
+        <v>0.2106387673746744</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1379,19 +1379,19 @@
         <v>40</v>
       </c>
       <c r="B36">
-        <v>1262598.486653646</v>
+        <v>1151851.8125</v>
       </c>
       <c r="C36">
-        <v>1.262598486653646</v>
+        <v>1.1518518125</v>
       </c>
       <c r="D36">
-        <v>1.028912063802083</v>
+        <v>0.9428332473958332</v>
       </c>
       <c r="E36">
-        <v>1.145755275227865</v>
+        <v>1.047342529947917</v>
       </c>
       <c r="F36">
-        <v>0.2864388188069661</v>
+        <v>0.2618356324869791</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1399,19 +1399,19 @@
         <v>41</v>
       </c>
       <c r="B37">
-        <v>1464948.033203125</v>
+        <v>1379126.861328125</v>
       </c>
       <c r="C37">
-        <v>1.464948033203125</v>
+        <v>1.379126861328125</v>
       </c>
       <c r="D37">
-        <v>1.262598486653646</v>
+        <v>1.1518518125</v>
       </c>
       <c r="E37">
-        <v>1.363773259928386</v>
+        <v>1.265489336914063</v>
       </c>
       <c r="F37">
-        <v>0.3409433149820963</v>
+        <v>0.3163723342285155</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1419,19 +1419,19 @@
         <v>42</v>
       </c>
       <c r="B38">
-        <v>1688063.014322917</v>
+        <v>1592190.266276042</v>
       </c>
       <c r="C38">
-        <v>1.688063014322917</v>
+        <v>1.592190266276042</v>
       </c>
       <c r="D38">
-        <v>1.464948033203125</v>
+        <v>1.379126861328125</v>
       </c>
       <c r="E38">
-        <v>1.576505523763021</v>
+        <v>1.485658563802083</v>
       </c>
       <c r="F38">
-        <v>0.3941263809407551</v>
+        <v>0.3714146409505208</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1439,19 +1439,19 @@
         <v>43</v>
       </c>
       <c r="B39">
-        <v>1903729.349609375</v>
+        <v>1791481.400390625</v>
       </c>
       <c r="C39">
-        <v>1.903729349609375</v>
+        <v>1.791481400390625</v>
       </c>
       <c r="D39">
-        <v>1.688063014322917</v>
+        <v>1.592190266276042</v>
       </c>
       <c r="E39">
-        <v>1.795896181966146</v>
+        <v>1.691835833333333</v>
       </c>
       <c r="F39">
-        <v>0.4489740454915365</v>
+        <v>0.4229589583333333</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1459,19 +1459,19 @@
         <v>44</v>
       </c>
       <c r="B40">
-        <v>2111411.909505208</v>
+        <v>1663421.220052083</v>
       </c>
       <c r="C40">
-        <v>2.111411909505208</v>
+        <v>1.663421220052083</v>
       </c>
       <c r="D40">
-        <v>1.903729349609375</v>
+        <v>1.791481400390625</v>
       </c>
       <c r="E40">
-        <v>2.007570629557291</v>
+        <v>1.727451310221354</v>
       </c>
       <c r="F40">
-        <v>0.5018926573893228</v>
+        <v>0.4318628275553384</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1479,19 +1479,19 @@
         <v>45</v>
       </c>
       <c r="B41">
-        <v>2301467.50390625</v>
+        <v>2149416.268229167</v>
       </c>
       <c r="C41">
-        <v>2.30146750390625</v>
+        <v>2.149416268229167</v>
       </c>
       <c r="D41">
-        <v>2.111411909505208</v>
+        <v>1.663421220052083</v>
       </c>
       <c r="E41">
-        <v>2.206439706705729</v>
+        <v>1.906418744140625</v>
       </c>
       <c r="F41">
-        <v>0.5516099266764323</v>
+        <v>0.4766046860351563</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1499,19 +1499,19 @@
         <v>46</v>
       </c>
       <c r="B42">
-        <v>2437485.73046875</v>
+        <v>2380722.126302083</v>
       </c>
       <c r="C42">
-        <v>2.43748573046875</v>
+        <v>2.380722126302083</v>
       </c>
       <c r="D42">
-        <v>2.30146750390625</v>
+        <v>2.149416268229167</v>
       </c>
       <c r="E42">
-        <v>2.3694766171875</v>
+        <v>2.265069197265625</v>
       </c>
       <c r="F42">
-        <v>0.592369154296875</v>
+        <v>0.5662672993164063</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1519,19 +1519,19 @@
         <v>47</v>
       </c>
       <c r="B43">
-        <v>2569529.276692708</v>
+        <v>2513382.825520833</v>
       </c>
       <c r="C43">
-        <v>2.569529276692708</v>
+        <v>2.513382825520833</v>
       </c>
       <c r="D43">
-        <v>2.43748573046875</v>
+        <v>2.380722126302083</v>
       </c>
       <c r="E43">
-        <v>2.503507503580729</v>
+        <v>2.447052475911458</v>
       </c>
       <c r="F43">
-        <v>0.6258768758951823</v>
+        <v>0.6117631189778645</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1539,19 +1539,19 @@
         <v>48</v>
       </c>
       <c r="B44">
-        <v>2716929.630208333</v>
+        <v>2610553.072916667</v>
       </c>
       <c r="C44">
-        <v>2.716929630208333</v>
+        <v>2.610553072916667</v>
       </c>
       <c r="D44">
-        <v>2.569529276692708</v>
+        <v>2.513382825520833</v>
       </c>
       <c r="E44">
-        <v>2.643229453450521</v>
+        <v>2.56196794921875</v>
       </c>
       <c r="F44">
-        <v>0.6608073633626301</v>
+        <v>0.6404919873046875</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1559,19 +1559,19 @@
         <v>49</v>
       </c>
       <c r="B45">
-        <v>2877964.766927083</v>
+        <v>2801555.65234375</v>
       </c>
       <c r="C45">
-        <v>2.877964766927083</v>
+        <v>2.80155565234375</v>
       </c>
       <c r="D45">
-        <v>2.716929630208333</v>
+        <v>2.610553072916667</v>
       </c>
       <c r="E45">
-        <v>2.797447198567709</v>
+        <v>2.706054362630208</v>
       </c>
       <c r="F45">
-        <v>0.699361799641927</v>
+        <v>0.676513590657552</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -1579,19 +1579,19 @@
         <v>50</v>
       </c>
       <c r="B46">
-        <v>2954226.1484375</v>
+        <v>2926482.61328125</v>
       </c>
       <c r="C46">
-        <v>2.9542261484375</v>
+        <v>2.92648261328125</v>
       </c>
       <c r="D46">
-        <v>2.877964766927083</v>
+        <v>2.80155565234375</v>
       </c>
       <c r="E46">
-        <v>2.916095457682292</v>
+        <v>2.8640191328125</v>
       </c>
       <c r="F46">
-        <v>0.7290238644205729</v>
+        <v>0.716004783203125</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -1599,19 +1599,19 @@
         <v>51</v>
       </c>
       <c r="B47">
-        <v>2937693.569010417</v>
+        <v>3064571.563802083</v>
       </c>
       <c r="C47">
-        <v>2.937693569010416</v>
+        <v>3.064571563802083</v>
       </c>
       <c r="D47">
-        <v>2.9542261484375</v>
+        <v>2.92648261328125</v>
       </c>
       <c r="E47">
-        <v>2.945959858723958</v>
+        <v>2.995527088541666</v>
       </c>
       <c r="F47">
-        <v>0.7364899646809895</v>
+        <v>0.7488817721354166</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -1619,19 +1619,19 @@
         <v>52</v>
       </c>
       <c r="B48">
-        <v>3020503.787760417</v>
+        <v>3145723.916666666</v>
       </c>
       <c r="C48">
-        <v>3.020503787760417</v>
+        <v>3.145723916666666</v>
       </c>
       <c r="D48">
-        <v>2.937693569010416</v>
+        <v>3.064571563802083</v>
       </c>
       <c r="E48">
-        <v>2.979098678385417</v>
+        <v>3.105147740234375</v>
       </c>
       <c r="F48">
-        <v>0.7447746695963542</v>
+        <v>0.7762869350585937</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -1639,19 +1639,19 @@
         <v>53</v>
       </c>
       <c r="B49">
-        <v>3196022.669270833</v>
+        <v>3282749.377604167</v>
       </c>
       <c r="C49">
-        <v>3.196022669270834</v>
+        <v>3.282749377604167</v>
       </c>
       <c r="D49">
-        <v>3.020503787760417</v>
+        <v>3.145723916666666</v>
       </c>
       <c r="E49">
-        <v>3.108263228515625</v>
+        <v>3.214236647135417</v>
       </c>
       <c r="F49">
-        <v>0.7770658071289062</v>
+        <v>0.803559161783854</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -1659,19 +1659,19 @@
         <v>54</v>
       </c>
       <c r="B50">
-        <v>3195557.708333333</v>
+        <v>3305515.59375</v>
       </c>
       <c r="C50">
-        <v>3.195557708333333</v>
+        <v>3.30551559375</v>
       </c>
       <c r="D50">
-        <v>3.196022669270834</v>
+        <v>3.282749377604167</v>
       </c>
       <c r="E50">
-        <v>3.195790188802083</v>
+        <v>3.294132485677084</v>
       </c>
       <c r="F50">
-        <v>0.7989475472005209</v>
+        <v>0.8235331214192709</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -1679,19 +1679,19 @@
         <v>55</v>
       </c>
       <c r="B51">
-        <v>3245345.85546875</v>
+        <v>3407572.5703125</v>
       </c>
       <c r="C51">
-        <v>3.24534585546875</v>
+        <v>3.4075725703125</v>
       </c>
       <c r="D51">
-        <v>3.195557708333333</v>
+        <v>3.30551559375</v>
       </c>
       <c r="E51">
-        <v>3.220451781901041</v>
+        <v>3.35654408203125</v>
       </c>
       <c r="F51">
-        <v>0.8051129454752602</v>
+        <v>0.8391360205078126</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -1699,19 +1699,19 @@
         <v>56</v>
       </c>
       <c r="B52">
-        <v>3225369.536458333</v>
+        <v>3442571.131510417</v>
       </c>
       <c r="C52">
-        <v>3.225369536458333</v>
+        <v>3.442571131510417</v>
       </c>
       <c r="D52">
-        <v>3.24534585546875</v>
+        <v>3.4075725703125</v>
       </c>
       <c r="E52">
-        <v>3.235357695963542</v>
+        <v>3.425071850911458</v>
       </c>
       <c r="F52">
-        <v>0.8088394239908854</v>
+        <v>0.8562679627278645</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -1719,19 +1719,19 @@
         <v>57</v>
       </c>
       <c r="B53">
-        <v>3313122.616536458</v>
+        <v>3497265.533854167</v>
       </c>
       <c r="C53">
-        <v>3.313122616536458</v>
+        <v>3.497265533854167</v>
       </c>
       <c r="D53">
-        <v>3.225369536458333</v>
+        <v>3.442571131510417</v>
       </c>
       <c r="E53">
-        <v>3.269246076497396</v>
+        <v>3.469918332682291</v>
       </c>
       <c r="F53">
-        <v>0.817311519124349</v>
+        <v>0.8674795831705728</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -1739,19 +1739,19 @@
         <v>58</v>
       </c>
       <c r="B54">
-        <v>0</v>
+        <v>3474681.3046875</v>
       </c>
       <c r="C54">
-        <v>0</v>
+        <v>3.4746813046875</v>
       </c>
       <c r="D54">
-        <v>3.313122616536458</v>
+        <v>3.497265533854167</v>
       </c>
       <c r="E54">
-        <v>1.656561308268229</v>
+        <v>3.485973419270833</v>
       </c>
       <c r="F54">
-        <v>0.4141403270670572</v>
+        <v>0.8714933548177082</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -1759,19 +1759,19 @@
         <v>59</v>
       </c>
       <c r="B55">
-        <v>0</v>
+        <v>3539855.645833333</v>
       </c>
       <c r="C55">
-        <v>0</v>
+        <v>3.539855645833333</v>
       </c>
       <c r="D55">
-        <v>0</v>
+        <v>3.4746813046875</v>
       </c>
       <c r="E55">
-        <v>0</v>
+        <v>3.507268475260417</v>
       </c>
       <c r="F55">
-        <v>0</v>
+        <v>0.8768171188151039</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -1779,19 +1779,19 @@
         <v>60</v>
       </c>
       <c r="B56">
-        <v>0</v>
+        <v>3445885.184895833</v>
       </c>
       <c r="C56">
-        <v>0</v>
+        <v>3.445885184895833</v>
       </c>
       <c r="D56">
-        <v>0</v>
+        <v>3.539855645833333</v>
       </c>
       <c r="E56">
-        <v>0</v>
+        <v>3.492870415364584</v>
       </c>
       <c r="F56">
-        <v>0</v>
+        <v>0.8732176038411457</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -1799,19 +1799,19 @@
         <v>61</v>
       </c>
       <c r="B57">
-        <v>0</v>
+        <v>3484593.58203125</v>
       </c>
       <c r="C57">
-        <v>0</v>
+        <v>3.48459358203125</v>
       </c>
       <c r="D57">
-        <v>0</v>
+        <v>3.445885184895833</v>
       </c>
       <c r="E57">
-        <v>0</v>
+        <v>3.465239383463541</v>
       </c>
       <c r="F57">
-        <v>0</v>
+        <v>0.8663098458658853</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -1819,19 +1819,19 @@
         <v>62</v>
       </c>
       <c r="B58">
-        <v>0</v>
+        <v>3515476.244791666</v>
       </c>
       <c r="C58">
-        <v>0</v>
+        <v>3.515476244791667</v>
       </c>
       <c r="D58">
-        <v>0</v>
+        <v>3.48459358203125</v>
       </c>
       <c r="E58">
-        <v>0</v>
+        <v>3.500034913411458</v>
       </c>
       <c r="F58">
-        <v>0</v>
+        <v>0.8750087283528645</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -1839,19 +1839,19 @@
         <v>63</v>
       </c>
       <c r="B59">
-        <v>0</v>
+        <v>3418572.27734375</v>
       </c>
       <c r="C59">
-        <v>0</v>
+        <v>3.41857227734375</v>
       </c>
       <c r="D59">
-        <v>0</v>
+        <v>3.515476244791667</v>
       </c>
       <c r="E59">
-        <v>0</v>
+        <v>3.467024261067708</v>
       </c>
       <c r="F59">
-        <v>0</v>
+        <v>0.8667560652669271</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -1859,19 +1859,19 @@
         <v>64</v>
       </c>
       <c r="B60">
-        <v>0</v>
+        <v>3361371</v>
       </c>
       <c r="C60">
-        <v>0</v>
+        <v>3.361371</v>
       </c>
       <c r="D60">
-        <v>0</v>
+        <v>3.41857227734375</v>
       </c>
       <c r="E60">
-        <v>0</v>
+        <v>3.389971638671875</v>
       </c>
       <c r="F60">
-        <v>0</v>
+        <v>0.8474929096679688</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -1885,13 +1885,13 @@
         <v>0</v>
       </c>
       <c r="D61">
-        <v>0</v>
+        <v>3.361371</v>
       </c>
       <c r="E61">
-        <v>0</v>
+        <v>1.6806855</v>
       </c>
       <c r="F61">
-        <v>0</v>
+        <v>0.420171375</v>
       </c>
     </row>
     <row r="62" spans="1:6">

</xml_diff>